<commit_message>
Adding an optional "non-global files" field.
Closes #96
</commit_message>
<xml_diff>
--- a/visium-no-probes/latest/visium-no-probes.xlsx
+++ b/visium-no-probes/latest/visium-no-probes.xlsx
@@ -159,6 +159,20 @@
     </comment>
     <comment ref="S1" authorId="1">
       <text>
+        <t>A semicolon separated list of non-shared files to be included in the dataset.
+The path assumes the files are located in the "TOP/non-global/" directory. For
+example, for the file is
+TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
+field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
+these files will be copied to the appropriate locations within the respective
+dataset directory tree. This field is used for internal HuBMAP processing.
+Examples for GeoMx and PhenoCycler are provided in the File Locations
+documentation:
+https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="1">
+      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -169,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="184">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -249,24 +263,24 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
   </si>
   <si>
-    <t>CosMx</t>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>SIMS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000202</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
   </si>
   <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
-    <t>SIMS</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000202</t>
-  </si>
-  <si>
     <t>Cell DIVE</t>
   </si>
   <si>
@@ -327,6 +341,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -687,6 +707,9 @@
     <t>https://identifiers.org/RRID:SCR_023732</t>
   </si>
   <si>
+    <t>non_global_files</t>
+  </si>
+  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -705,7 +728,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-04-24T10:54:03-07:00</t>
+    <t>2025-06-16T16:44:00-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -764,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -788,6 +811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -798,7 +822,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -822,7 +846,8 @@
     <col min="16" max="16" style="17" width="21.80078125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" style="18" width="25.0859375" customWidth="true" bestFit="true"/>
     <col min="18" max="18" style="19" width="24.57421875" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="16.91796875" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" style="20" width="13.33984375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" style="21" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -839,63 +864,66 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>172</v>
+        <v>174</v>
+      </c>
+      <c r="T1" t="s" s="1">
+        <v>175</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="S2" t="s" s="20">
-        <v>173</v>
+      <c r="T2" t="s" s="21">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="13">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$42</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -961,16 +989,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2">
@@ -978,13 +1006,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -994,7 +1022,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1326,6 +1354,14 @@
       </c>
       <c r="B41" t="s" s="0">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1343,18 +1379,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1372,18 +1408,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1401,10 +1437,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1422,62 +1458,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1495,10 +1531,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1516,74 +1552,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1601,146 +1637,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating other Visium templates
</commit_message>
<xml_diff>
--- a/visium-no-probes/latest/visium-no-probes.xlsx
+++ b/visium-no-probes/latest/visium-no-probes.xlsx
@@ -83,13 +83,13 @@
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>For Visium, this is the area of spots that was covered by tissue within the
-captured area, not the total possible captured area which is fixed. For GeoMx
-this would be the area of the AOI being captured. For HiFi this is the summed
-area of the ROIs in a single flowcell lane. For CosMx and Resolve, this is the
-area of the FOV (aka ROI) region being captured. For Xenium this is the total
-area of the FOV regions (aka ROI) being captured. For Stereo-Seq this is the
-number of beads.</t>
+        <t>(Required) For Visium, this is the area of spots that was covered by tissue
+within the captured area, not the total possible captured area which is fixed.
+For GeoMx this would be the area of the AOI being captured. For HiFi this is the
+summed area of the ROIs in a single flowcell lane. For CosMx and Resolve, this
+is the area of the FOV (aka ROI) region being captured. For Xenium this is the
+total area of the FOV regions (aka ROI) being captured. For Stereo-Seq this is
+the number of beads.</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="198">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -209,34 +209,166 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
   </si>
   <si>
     <t>Xenium</t>
@@ -245,42 +377,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000202</t>
   </si>
   <si>
-    <t>CosMx Transcriptomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
     <t>Cell DIVE</t>
   </si>
   <si>
@@ -305,16 +407,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -323,30 +419,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -377,18 +455,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -401,12 +467,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -419,34 +479,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>contributors_path</t>
@@ -728,7 +770,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-06-16T16:44:00-07:00</t>
+    <t>2025-08-15T09:10:26-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -864,66 +906,66 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T2" t="s" s="21">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="13">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$42</formula1>
+      <formula1>'dataset_type'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -989,30 +1031,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -1022,7 +1064,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1362,6 +1404,62 @@
       </c>
       <c r="B42" t="s" s="0">
         <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1379,18 +1477,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>93</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1408,18 +1506,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>93</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1437,10 +1535,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1458,62 +1556,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>111</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1531,10 +1629,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1552,74 +1650,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1637,146 +1735,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>145</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>149</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>151</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>155</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>157</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>161</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>163</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>169</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>171</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>